<commit_message>
pres poll 20201011 clean data and data dictionary update
upload of cleaned pres polls 20201011 data via Mr Data, and added data dictionay info into data dictionary file
</commit_message>
<xml_diff>
--- a/data/clean_data/data_dictionary.xlsx
+++ b/data/clean_data/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Desktop\us-elections\data\clean_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6FE27504-5845-471F-9608-5F542EDF256D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08B4530-2955-4BBB-B72E-E132C0606365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="presidential_national_toplines" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="123">
   <si>
     <t>Description</t>
   </si>
@@ -348,12 +348,60 @@
   </si>
   <si>
     <t>state_cen</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Len</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>Dem</t>
+  </si>
+  <si>
+    <t>GOP</t>
+  </si>
+  <si>
+    <t>Ind</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Pollster</t>
+  </si>
+  <si>
+    <t>Day of the year at the midpoint of the poll - so a poll from Feb 02 to Feb 04 would have Feb 03 as the midpoint and this is day 34</t>
+  </si>
+  <si>
+    <t>Duration of Poll</t>
+  </si>
+  <si>
+    <t>Electoral Vote</t>
+  </si>
+  <si>
+    <t>Democrat Party %</t>
+  </si>
+  <si>
+    <t>Republican Party %</t>
+  </si>
+  <si>
+    <t>Independent Party %</t>
+  </si>
+  <si>
+    <t>End-date of data collection for poll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="11"/>
@@ -1196,7 +1244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1383,7 +1431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1519,7 +1567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1634,7 +1682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1829,7 +1877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1880,7 +1928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2019,11 +2067,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2039,16 +2087,88 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>